<commit_message>
fixed pq, endless loop, hardcoded childhood lang
</commit_message>
<xml_diff>
--- a/experiment_implementation/data/participant_questionnaire_toy_x_1/language_iso639_1_toy.xlsx
+++ b/experiment_implementation/data/participant_questionnaire_toy_x_1/language_iso639_1_toy.xlsx
@@ -1,21 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C748E6C5-359C-4E4F-B3FB-6ED9B78F0904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="language_iso639_1_en" sheetId="1" r:id="rId1"/>
+    <sheet name="language_iso639_1_en" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -163,7 +156,7 @@
     <t>ca</t>
   </si>
   <si>
-    <t>Catalan, Valencian</t>
+    <t xml:space="preserve">Catalan, Valencian</t>
   </si>
   <si>
     <t>ce</t>
@@ -199,7 +192,7 @@
     <t>cu</t>
   </si>
   <si>
-    <t>Church Slavic, Old Slavonic, Church Slavonic, Old Bulgarian, Old Church Slavonic</t>
+    <t xml:space="preserve">Church Slavic, Old Slavonic, Church Slavonic, Old Bulgarian, Old Church Slavonic</t>
   </si>
   <si>
     <t>cv</t>
@@ -229,7 +222,7 @@
     <t>dv</t>
   </si>
   <si>
-    <t>Divehi, Dhivehi, Maldivian</t>
+    <t xml:space="preserve">Divehi, Dhivehi, Maldivian</t>
   </si>
   <si>
     <t>dz</t>
@@ -247,7 +240,7 @@
     <t>el</t>
   </si>
   <si>
-    <t>Modern Greek</t>
+    <t xml:space="preserve">Modern Greek</t>
   </si>
   <si>
     <t>en</t>
@@ -265,7 +258,7 @@
     <t>es</t>
   </si>
   <si>
-    <t>Spanish, Castilian</t>
+    <t xml:space="preserve">Spanish, Castilian</t>
   </si>
   <si>
     <t>et</t>
@@ -319,7 +312,7 @@
     <t>fy</t>
   </si>
   <si>
-    <t>Western Frisian</t>
+    <t xml:space="preserve">Western Frisian</t>
   </si>
   <si>
     <t>ga</t>
@@ -331,7 +324,7 @@
     <t>gd</t>
   </si>
   <si>
-    <t>Gaelic, Scottish Gaelic</t>
+    <t xml:space="preserve">Gaelic, Scottish Gaelic</t>
   </si>
   <si>
     <t>gl</t>
@@ -367,7 +360,7 @@
     <t>he</t>
   </si>
   <si>
-    <t>Modern Hebrew</t>
+    <t xml:space="preserve">Modern Hebrew</t>
   </si>
   <si>
     <t>hi</t>
@@ -379,7 +372,7 @@
     <t>ho</t>
   </si>
   <si>
-    <t>Hiri Motu</t>
+    <t xml:space="preserve">Hiri Motu</t>
   </si>
   <si>
     <t>hr</t>
@@ -391,7 +384,7 @@
     <t>ht</t>
   </si>
   <si>
-    <t>Haitian, Haitian Creole</t>
+    <t xml:space="preserve">Haitian, Haitian Creole</t>
   </si>
   <si>
     <t>hu</t>
@@ -415,7 +408,7 @@
     <t>ia</t>
   </si>
   <si>
-    <t>Interlingua (International Auxiliary Language Association)</t>
+    <t xml:space="preserve">Interlingua (International Auxiliary Language Association)</t>
   </si>
   <si>
     <t>id</t>
@@ -427,7 +420,7 @@
     <t>ie</t>
   </si>
   <si>
-    <t>Interlingue, Occidental</t>
+    <t xml:space="preserve">Interlingue, Occidental</t>
   </si>
   <si>
     <t>ig</t>
@@ -439,7 +432,7 @@
     <t>ii</t>
   </si>
   <si>
-    <t>Sichuan Yi, Nuosu</t>
+    <t xml:space="preserve">Sichuan Yi, Nuosu</t>
   </si>
   <si>
     <t>ik</t>
@@ -499,13 +492,13 @@
     <t>ki</t>
   </si>
   <si>
-    <t>Kikuyu, Gikuyu</t>
+    <t xml:space="preserve">Kikuyu, Gikuyu</t>
   </si>
   <si>
     <t>kj</t>
   </si>
   <si>
-    <t>Kwanyama, Kuanyama</t>
+    <t xml:space="preserve">Kwanyama, Kuanyama</t>
   </si>
   <si>
     <t>kk</t>
@@ -517,13 +510,13 @@
     <t>kl</t>
   </si>
   <si>
-    <t>Kalaallisut, Greenlandic</t>
+    <t xml:space="preserve">Kalaallisut, Greenlandic</t>
   </si>
   <si>
     <t>km</t>
   </si>
   <si>
-    <t>Central Khmer</t>
+    <t xml:space="preserve">Central Khmer</t>
   </si>
   <si>
     <t>kn</t>
@@ -571,7 +564,7 @@
     <t>ky</t>
   </si>
   <si>
-    <t>Kirghiz, Kyrgyz</t>
+    <t xml:space="preserve">Kirghiz, Kyrgyz</t>
   </si>
   <si>
     <t>la</t>
@@ -583,7 +576,7 @@
     <t>lb</t>
   </si>
   <si>
-    <t>Luxembourgish, Letzeburgesch</t>
+    <t xml:space="preserve">Luxembourgish, Letzeburgesch</t>
   </si>
   <si>
     <t>lg</t>
@@ -595,7 +588,7 @@
     <t>li</t>
   </si>
   <si>
-    <t>Limburgish, Limburgan, Limburger</t>
+    <t xml:space="preserve">Limburgish, Limburgan, Limburger</t>
   </si>
   <si>
     <t>ln</t>
@@ -646,7 +639,7 @@
     <t>Māori</t>
   </si>
   <si>
-    <t>mk / sl</t>
+    <t xml:space="preserve">mk / sl</t>
   </si>
   <si>
     <t>Macedonian</t>
@@ -703,13 +696,13 @@
     <t>nb</t>
   </si>
   <si>
-    <t>Norwegian Bokmål</t>
+    <t xml:space="preserve">Norwegian Bokmål</t>
   </si>
   <si>
     <t>nd</t>
   </si>
   <si>
-    <t>North Ndebele</t>
+    <t xml:space="preserve">North Ndebele</t>
   </si>
   <si>
     <t>ne</t>
@@ -727,13 +720,13 @@
     <t>nl</t>
   </si>
   <si>
-    <t>Dutch, Flemish</t>
+    <t xml:space="preserve">Dutch, Flemish</t>
   </si>
   <si>
     <t>nn</t>
   </si>
   <si>
-    <t>Norwegian Nynorsk</t>
+    <t xml:space="preserve">Norwegian Nynorsk</t>
   </si>
   <si>
     <t>no</t>
@@ -745,25 +738,25 @@
     <t>nr</t>
   </si>
   <si>
-    <t>South Ndebele</t>
+    <t xml:space="preserve">South Ndebele</t>
   </si>
   <si>
     <t>nv</t>
   </si>
   <si>
-    <t>Navajo, Navaho</t>
+    <t xml:space="preserve">Navajo, Navaho</t>
   </si>
   <si>
     <t>ny</t>
   </si>
   <si>
-    <t>Chichewa, Chewa, Nyanja</t>
+    <t xml:space="preserve">Chichewa, Chewa, Nyanja</t>
   </si>
   <si>
     <t>oc</t>
   </si>
   <si>
-    <t>Occitan (after 1500)</t>
+    <t xml:space="preserve">Occitan (after 1500)</t>
   </si>
   <si>
     <t>oj</t>
@@ -787,13 +780,13 @@
     <t>os</t>
   </si>
   <si>
-    <t>Ossetian, Ossetic</t>
+    <t xml:space="preserve">Ossetian, Ossetic</t>
   </si>
   <si>
     <t>pa</t>
   </si>
   <si>
-    <t>Panjabi, Punjabi</t>
+    <t xml:space="preserve">Panjabi, Punjabi</t>
   </si>
   <si>
     <t>pi</t>
@@ -811,7 +804,7 @@
     <t>ps</t>
   </si>
   <si>
-    <t>Pashto, Pushto</t>
+    <t xml:space="preserve">Pashto, Pushto</t>
   </si>
   <si>
     <t>pt</t>
@@ -841,7 +834,7 @@
     <t>ro</t>
   </si>
   <si>
-    <t>Romanian, Moldavian, Moldovan</t>
+    <t xml:space="preserve">Romanian, Moldavian, Moldovan</t>
   </si>
   <si>
     <t>ru</t>
@@ -877,7 +870,7 @@
     <t>se</t>
   </si>
   <si>
-    <t>Northern Sami</t>
+    <t xml:space="preserve">Northern Sami</t>
   </si>
   <si>
     <t>sg</t>
@@ -895,7 +888,7 @@
     <t>si</t>
   </si>
   <si>
-    <t>Sinhala, Sinhalese</t>
+    <t xml:space="preserve">Sinhala, Sinhalese</t>
   </si>
   <si>
     <t>sk</t>
@@ -949,7 +942,7 @@
     <t>st</t>
   </si>
   <si>
-    <t>Southern Sotho</t>
+    <t xml:space="preserve">Southern Sotho</t>
   </si>
   <si>
     <t>su</t>
@@ -1021,7 +1014,7 @@
     <t>to</t>
   </si>
   <si>
-    <t>Tonga (Tonga Islands)</t>
+    <t xml:space="preserve">Tonga (Tonga Islands)</t>
   </si>
   <si>
     <t>tr</t>
@@ -1057,7 +1050,7 @@
     <t>ug</t>
   </si>
   <si>
-    <t>Uighur, Uyghur</t>
+    <t xml:space="preserve">Uighur, Uyghur</t>
   </si>
   <si>
     <t>uk</t>
@@ -1129,7 +1122,7 @@
     <t>za</t>
   </si>
   <si>
-    <t>Zhuang, Chuang</t>
+    <t xml:space="preserve">Zhuang, Chuang</t>
   </si>
   <si>
     <t>zh</t>
@@ -1147,141 +1140,122 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11.000000"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.000000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.000000"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.000000"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18.000000"/>
       <color theme="3"/>
       <name val="Aptos Display"/>
-      <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11.000000"/>
+      <color indexed="2"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1293,47 +1267,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1345,24 +1309,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1374,41 +1351,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1420,41 +1363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1464,41 +1373,92 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -1513,7 +1473,73 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -1528,149 +1554,113 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="none"/>
+      <right style="none"/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="14" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="15" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="16" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="17" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="18" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="20" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="21" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="22" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="23" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="24" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="25" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="2" fillId="26" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="3" fillId="27" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
+    <xf fontId="4" fillId="28" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="6" fillId="29" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="7" fillId="0" borderId="3" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
+    <xf fontId="8" fillId="0" borderId="4" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
+    <xf fontId="9" fillId="0" borderId="5" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="10" fillId="30" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
+    <xf fontId="11" fillId="0" borderId="6" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
+    <xf fontId="12" fillId="31" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="32" borderId="7" numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1" applyProtection="0"/>
+    <xf fontId="13" fillId="27" borderId="8" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
+    <xf fontId="14" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="15" fillId="0" borderId="9" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
+    <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53"/>
+    <cellStyle name="Good" xfId="29" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19"/>
+    <cellStyle name="Input" xfId="34" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="37" builtinId="10"/>
+    <cellStyle name="Output" xfId="38" builtinId="21"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Total" xfId="40" builtinId="25"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1678,15 +1668,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1728,108 +1998,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Aptos Display"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Aptos Narrow"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1837,7 +2013,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1863,7 +2039,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1915,16 +2091,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1940,7 +2128,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1972,7 +2160,7 @@
   </a:themeElements>
   <a:objectDefaults>
     <a:lnDef>
-      <a:spPr/>
+      <a:spPr bwMode="auto"/>
       <a:bodyPr/>
       <a:lstStyle/>
       <a:style>
@@ -1991,24 +2179,23 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="19.75390625"/>
+    <col customWidth="1" min="2" max="2" width="70.75390625"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2016,15 +2203,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2032,7 +2219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2040,7 +2227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2048,7 +2235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2056,7 +2243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2064,7 +2251,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2072,7 +2259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2080,7 +2267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2088,7 +2275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2096,7 +2283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2104,7 +2291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2120,7 +2307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2128,7 +2315,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2136,7 +2323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2144,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2152,7 +2339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2160,7 +2347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2168,7 +2355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2176,7 +2363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2184,7 +2371,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2192,7 +2379,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2208,7 +2395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2216,7 +2403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2224,7 +2411,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2232,7 +2419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2240,7 +2427,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2248,7 +2435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -2256,7 +2443,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -2264,7 +2451,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -2272,7 +2459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2280,7 +2467,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2288,7 +2475,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -2296,7 +2483,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2304,7 +2491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -2312,7 +2499,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2320,7 +2507,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2328,7 +2515,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2336,7 +2523,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2344,7 +2531,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -2352,7 +2539,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2360,7 +2547,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2368,7 +2555,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2376,7 +2563,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -2384,7 +2571,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2392,7 +2579,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -2400,7 +2587,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2408,7 +2595,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -2416,7 +2603,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -2424,7 +2611,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -2432,7 +2619,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -2440,7 +2627,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -2448,7 +2635,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -2456,7 +2643,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2464,7 +2651,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -2472,7 +2659,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -2480,7 +2667,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -2488,7 +2675,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -2496,7 +2683,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -2504,7 +2691,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2512,7 +2699,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -2520,7 +2707,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -2528,7 +2715,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -2536,7 +2723,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -2544,7 +2731,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -2552,7 +2739,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -2560,7 +2747,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -2568,7 +2755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -2576,7 +2763,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -2584,7 +2771,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -2592,7 +2779,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -2600,7 +2787,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -2608,7 +2795,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -2616,7 +2803,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -2624,7 +2811,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -2632,7 +2819,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -2640,7 +2827,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -2648,7 +2835,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81">
       <c r="A81" t="s">
         <v>160</v>
       </c>
@@ -2656,7 +2843,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -2664,7 +2851,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -2672,7 +2859,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -2680,7 +2867,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85">
       <c r="A85" t="s">
         <v>168</v>
       </c>
@@ -2688,7 +2875,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86">
       <c r="A86" t="s">
         <v>170</v>
       </c>
@@ -2696,7 +2883,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -2704,7 +2891,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -2712,7 +2899,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -2720,7 +2907,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90">
       <c r="A90" t="s">
         <v>178</v>
       </c>
@@ -2728,7 +2915,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -2736,7 +2923,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92">
       <c r="A92" t="s">
         <v>182</v>
       </c>
@@ -2744,7 +2931,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -2752,7 +2939,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -2760,7 +2947,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -2768,7 +2955,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -2776,7 +2963,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97">
       <c r="A97" t="s">
         <v>192</v>
       </c>
@@ -2784,7 +2971,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98">
       <c r="A98" t="s">
         <v>194</v>
       </c>
@@ -2792,7 +2979,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -2800,7 +2987,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100">
       <c r="A100" t="s">
         <v>198</v>
       </c>
@@ -2808,7 +2995,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101">
       <c r="A101" t="s">
         <v>200</v>
       </c>
@@ -2816,7 +3003,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -2824,7 +3011,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -2832,7 +3019,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104">
       <c r="A104" t="s">
         <v>206</v>
       </c>
@@ -2840,7 +3027,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105">
       <c r="A105" t="s">
         <v>208</v>
       </c>
@@ -2848,7 +3035,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106">
       <c r="A106" t="s">
         <v>210</v>
       </c>
@@ -2856,7 +3043,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107">
       <c r="A107" t="s">
         <v>212</v>
       </c>
@@ -2864,7 +3051,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108">
       <c r="A108" t="s">
         <v>214</v>
       </c>
@@ -2872,7 +3059,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109">
       <c r="A109" t="s">
         <v>216</v>
       </c>
@@ -2880,7 +3067,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110">
       <c r="A110" t="s">
         <v>218</v>
       </c>
@@ -2888,7 +3075,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111">
       <c r="A111" t="s">
         <v>220</v>
       </c>
@@ -2896,7 +3083,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -2904,7 +3091,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113">
       <c r="A113" t="s">
         <v>224</v>
       </c>
@@ -2912,7 +3099,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114">
       <c r="A114" t="s">
         <v>226</v>
       </c>
@@ -2920,7 +3107,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115">
       <c r="A115" t="s">
         <v>228</v>
       </c>
@@ -2928,7 +3115,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116">
       <c r="A116" t="s">
         <v>230</v>
       </c>
@@ -2936,7 +3123,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -2944,7 +3131,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118">
       <c r="A118" t="s">
         <v>234</v>
       </c>
@@ -2952,7 +3139,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119">
       <c r="A119" t="s">
         <v>236</v>
       </c>
@@ -2960,7 +3147,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120">
       <c r="A120" t="s">
         <v>238</v>
       </c>
@@ -2968,7 +3155,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121">
       <c r="A121" t="s">
         <v>240</v>
       </c>
@@ -2976,7 +3163,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -2984,7 +3171,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123">
       <c r="A123" t="s">
         <v>244</v>
       </c>
@@ -2992,7 +3179,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124">
       <c r="A124" t="s">
         <v>246</v>
       </c>
@@ -3000,7 +3187,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -3008,7 +3195,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126">
       <c r="A126" t="s">
         <v>250</v>
       </c>
@@ -3016,7 +3203,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127">
       <c r="A127" t="s">
         <v>252</v>
       </c>
@@ -3024,7 +3211,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -3032,7 +3219,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -3040,7 +3227,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130">
       <c r="A130" t="s">
         <v>258</v>
       </c>
@@ -3048,7 +3235,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131">
       <c r="A131" t="s">
         <v>260</v>
       </c>
@@ -3056,7 +3243,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -3064,7 +3251,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133">
       <c r="A133" t="s">
         <v>264</v>
       </c>
@@ -3072,7 +3259,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134">
       <c r="A134" t="s">
         <v>266</v>
       </c>
@@ -3080,7 +3267,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135">
       <c r="A135" t="s">
         <v>268</v>
       </c>
@@ -3088,7 +3275,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -3096,7 +3283,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137">
       <c r="A137" t="s">
         <v>272</v>
       </c>
@@ -3104,7 +3291,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138">
       <c r="A138" t="s">
         <v>274</v>
       </c>
@@ -3112,7 +3299,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139">
       <c r="A139" t="s">
         <v>276</v>
       </c>
@@ -3120,7 +3307,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -3128,7 +3315,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141">
       <c r="A141" t="s">
         <v>280</v>
       </c>
@@ -3136,7 +3323,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142">
       <c r="A142" t="s">
         <v>282</v>
       </c>
@@ -3144,7 +3331,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143">
       <c r="A143" t="s">
         <v>284</v>
       </c>
@@ -3152,7 +3339,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144">
       <c r="A144" t="s">
         <v>286</v>
       </c>
@@ -3160,7 +3347,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145">
       <c r="A145" t="s">
         <v>288</v>
       </c>
@@ -3168,7 +3355,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146">
       <c r="A146" t="s">
         <v>290</v>
       </c>
@@ -3176,7 +3363,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147">
       <c r="A147" t="s">
         <v>292</v>
       </c>
@@ -3184,7 +3371,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148">
       <c r="A148" t="s">
         <v>294</v>
       </c>
@@ -3192,7 +3379,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149">
       <c r="A149" t="s">
         <v>296</v>
       </c>
@@ -3200,7 +3387,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150">
       <c r="A150" t="s">
         <v>298</v>
       </c>
@@ -3208,7 +3395,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151">
       <c r="A151" t="s">
         <v>300</v>
       </c>
@@ -3216,7 +3403,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152">
       <c r="A152" t="s">
         <v>302</v>
       </c>
@@ -3224,7 +3411,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153">
       <c r="A153" t="s">
         <v>304</v>
       </c>
@@ -3232,7 +3419,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154">
       <c r="A154" t="s">
         <v>306</v>
       </c>
@@ -3240,7 +3427,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155">
       <c r="A155" t="s">
         <v>308</v>
       </c>
@@ -3248,7 +3435,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156">
       <c r="A156" t="s">
         <v>310</v>
       </c>
@@ -3256,7 +3443,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157">
       <c r="A157" t="s">
         <v>312</v>
       </c>
@@ -3264,7 +3451,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158">
       <c r="A158" t="s">
         <v>314</v>
       </c>
@@ -3272,7 +3459,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159">
       <c r="A159" t="s">
         <v>316</v>
       </c>
@@ -3280,7 +3467,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160">
       <c r="A160" t="s">
         <v>318</v>
       </c>
@@ -3288,7 +3475,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161">
       <c r="A161" t="s">
         <v>320</v>
       </c>
@@ -3296,7 +3483,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162">
       <c r="A162" t="s">
         <v>322</v>
       </c>
@@ -3304,7 +3491,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163">
       <c r="A163" t="s">
         <v>324</v>
       </c>
@@ -3312,7 +3499,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164">
       <c r="A164" t="s">
         <v>326</v>
       </c>
@@ -3320,7 +3507,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165">
       <c r="A165" t="s">
         <v>328</v>
       </c>
@@ -3328,7 +3515,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166">
       <c r="A166" t="s">
         <v>330</v>
       </c>
@@ -3336,7 +3523,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167">
       <c r="A167" t="s">
         <v>332</v>
       </c>
@@ -3344,7 +3531,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168">
       <c r="A168" t="s">
         <v>334</v>
       </c>
@@ -3352,7 +3539,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169">
       <c r="A169" t="s">
         <v>336</v>
       </c>
@@ -3360,7 +3547,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170">
       <c r="A170" t="s">
         <v>338</v>
       </c>
@@ -3368,7 +3555,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171">
       <c r="A171" t="s">
         <v>340</v>
       </c>
@@ -3376,7 +3563,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172">
       <c r="A172" t="s">
         <v>342</v>
       </c>
@@ -3384,7 +3571,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173">
       <c r="A173" t="s">
         <v>344</v>
       </c>
@@ -3392,7 +3579,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174">
       <c r="A174" t="s">
         <v>346</v>
       </c>
@@ -3400,7 +3587,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175">
       <c r="A175" t="s">
         <v>348</v>
       </c>
@@ -3408,7 +3595,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176">
       <c r="A176" t="s">
         <v>350</v>
       </c>
@@ -3416,7 +3603,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177">
       <c r="A177" t="s">
         <v>352</v>
       </c>
@@ -3424,7 +3611,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178">
       <c r="A178" t="s">
         <v>354</v>
       </c>
@@ -3432,7 +3619,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -3440,7 +3627,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180">
       <c r="A180" t="s">
         <v>358</v>
       </c>
@@ -3448,7 +3635,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181">
       <c r="A181" t="s">
         <v>360</v>
       </c>
@@ -3456,7 +3643,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -3464,7 +3651,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183">
       <c r="A183" t="s">
         <v>364</v>
       </c>
@@ -3472,7 +3659,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184">
       <c r="A184" t="s">
         <v>366</v>
       </c>
@@ -3480,7 +3667,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185">
       <c r="A185" t="s">
         <v>368</v>
       </c>
@@ -3488,7 +3675,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186">
       <c r="A186" t="s">
         <v>370</v>
       </c>
@@ -3496,7 +3683,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187">
       <c r="A187" t="s">
         <v>372</v>
       </c>
@@ -3505,6 +3692,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>